<commit_message>
update results excel file
</commit_message>
<xml_diff>
--- a/collocation_results.xlsx
+++ b/collocation_results.xlsx
@@ -14,17 +14,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="129">
   <si>
     <t>ex1ocp</t>
   </si>
   <si>
-    <t>sequential</t>
-  </si>
-  <si>
-    <t>4cores</t>
-  </si>
-  <si>
     <t>ex2ocp</t>
   </si>
   <si>
@@ -395,6 +389,18 @@
   </si>
   <si>
     <t>exnc2ocp</t>
+  </si>
+  <si>
+    <t>sequential-101nodes</t>
+  </si>
+  <si>
+    <t>4cores-101nodes</t>
+  </si>
+  <si>
+    <t>sequential-501nodes</t>
+  </si>
+  <si>
+    <t>4cores-501nodes</t>
   </si>
 </sst>
 </file>
@@ -737,28 +743,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C127"/>
+  <dimension ref="A1:E127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="E125" sqref="E125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.28515625" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
+    <col min="4" max="4" width="24.140625" customWidth="1"/>
+    <col min="5" max="5" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>1</v>
+        <v>125</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+      <c r="D1" t="s">
+        <v>127</v>
+      </c>
+      <c r="E1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -768,10 +782,16 @@
       <c r="C2" s="1">
         <v>7.9942140000000004</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="1">
+        <v>20.02966</v>
+      </c>
+      <c r="E2" s="1">
+        <v>18.412179999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B3" s="1">
         <v>0.40797909999999998</v>
@@ -779,10 +799,16 @@
       <c r="C3" s="1">
         <v>0.56112359999999994</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" s="1">
+        <v>1.463759</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1.445246</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B4" s="1">
         <v>63.080910000000003</v>
@@ -790,10 +816,16 @@
       <c r="C4" s="1">
         <v>70.368039999999993</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" s="1">
+        <v>288.17230000000001</v>
+      </c>
+      <c r="E4" s="1">
+        <v>225.72329999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B5" s="1">
         <v>68.925539999999998</v>
@@ -802,9 +834,9 @@
         <v>94.553330000000003</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B6" s="1">
         <v>67.082220000000007</v>
@@ -812,10 +844,16 @@
       <c r="C6" s="1">
         <v>80.9465</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" s="1">
+        <v>313.73950000000002</v>
+      </c>
+      <c r="E6" s="1">
+        <v>248.9375</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B7" s="1">
         <v>63.710909999999998</v>
@@ -823,10 +861,16 @@
       <c r="C7" s="1">
         <v>72.137789999999995</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" s="1">
+        <v>291.50360000000001</v>
+      </c>
+      <c r="E7" s="1">
+        <v>225.90170000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B8" s="1">
         <v>32.314390000000003</v>
@@ -834,10 +878,11 @@
       <c r="C8" s="1">
         <v>37.132330000000003</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B9" s="1">
         <v>81.057199999999995</v>
@@ -845,10 +890,16 @@
       <c r="C9" s="1">
         <v>86.385270000000006</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" s="1">
+        <v>366.67410000000001</v>
+      </c>
+      <c r="E9" s="1">
+        <v>344.46910000000003</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B10" s="1">
         <v>0.96370330000000004</v>
@@ -856,15 +907,27 @@
       <c r="C10" s="1">
         <v>1.252006</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" s="1">
+        <v>7.4540660000000001</v>
+      </c>
+      <c r="E10" s="1">
+        <v>4.2074369999999996</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="D11" s="1">
+        <v>3.759919</v>
+      </c>
+      <c r="E11" s="1">
+        <v>3.3247640000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B12" s="1">
         <v>52.320799999999998</v>
@@ -872,10 +935,16 @@
       <c r="C12" s="1">
         <v>61.804470000000002</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12" s="1">
+        <v>296.49689999999998</v>
+      </c>
+      <c r="E12" s="1">
+        <v>240.11089999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B13" s="1">
         <v>855.94860000000006</v>
@@ -883,10 +952,11 @@
       <c r="C13" s="1">
         <v>765.88059999999996</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B14" s="1">
         <v>0.36630109999999999</v>
@@ -894,17 +964,23 @@
       <c r="C14" s="1">
         <v>0.63878369999999995</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14" s="1">
+        <v>1.485744</v>
+      </c>
+      <c r="E14" s="1">
+        <v>1.4476370000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B16" s="1">
         <v>155.1122</v>
@@ -912,10 +988,16 @@
       <c r="C16" s="1">
         <v>186.48220000000001</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" s="1">
+        <v>941.42240000000004</v>
+      </c>
+      <c r="E16" s="1">
+        <v>835.12080000000003</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B17" s="1">
         <v>53.426389999999998</v>
@@ -923,10 +1005,16 @@
       <c r="C17" s="1">
         <v>58.725490000000001</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17" s="1">
+        <v>234.4897</v>
+      </c>
+      <c r="E17" s="1">
+        <v>205.76740000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B18" s="1">
         <v>3.099313</v>
@@ -934,10 +1022,16 @@
       <c r="C18" s="1">
         <v>5.108746</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18" s="1">
+        <v>17.952279999999998</v>
+      </c>
+      <c r="E18" s="1">
+        <v>15.27788</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B19" s="1">
         <v>1172.3530000000001</v>
@@ -946,9 +1040,9 @@
         <v>1673.877</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B20" s="1">
         <v>3.527533</v>
@@ -956,15 +1050,21 @@
       <c r="C20" s="1">
         <v>4.2598130000000003</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20" s="1">
+        <v>9.6181909999999995</v>
+      </c>
+      <c r="E20" s="1">
+        <v>7.6727869999999996</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B22" s="1">
         <v>2.2515779999999999</v>
@@ -972,10 +1072,16 @@
       <c r="C22" s="1">
         <v>2.5185689999999998</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22" s="1">
+        <v>9.4240639999999996</v>
+      </c>
+      <c r="E22" s="1">
+        <v>7.8332959999999998</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B23" s="1">
         <v>160.85079999999999</v>
@@ -983,10 +1089,16 @@
       <c r="C23" s="1">
         <v>220.3552</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23" s="1">
+        <v>783.15239999999994</v>
+      </c>
+      <c r="E23" s="1">
+        <v>1005.513</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B24" s="1">
         <v>2.9142320000000002</v>
@@ -994,15 +1106,21 @@
       <c r="C24" s="1">
         <v>3.8134009999999998</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24" s="1">
+        <v>15.487259999999999</v>
+      </c>
+      <c r="E24" s="1">
+        <v>11.753209999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B26" s="1">
         <v>2.950628</v>
@@ -1010,10 +1128,16 @@
       <c r="C26" s="1">
         <v>5.0400150000000004</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D26" s="1">
+        <v>13.81695</v>
+      </c>
+      <c r="E26" s="1">
+        <v>20.16947</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B27" s="1">
         <v>3.4607320000000001</v>
@@ -1021,15 +1145,27 @@
       <c r="C27" s="1">
         <v>4.8464919999999996</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D27" s="1">
+        <v>18.30246</v>
+      </c>
+      <c r="E27" s="1">
+        <v>19.34704</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="D28" s="1">
+        <v>402.55399999999997</v>
+      </c>
+      <c r="E28" s="1">
+        <v>588.005</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B29" s="1">
         <v>2.2973659999999998</v>
@@ -1037,10 +1173,16 @@
       <c r="C29" s="1">
         <v>5.0242069999999996</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D29" s="1">
+        <v>12.06019</v>
+      </c>
+      <c r="E29" s="1">
+        <v>11.50037</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B30" s="1">
         <v>108.11969999999999</v>
@@ -1048,10 +1190,16 @@
       <c r="C30" s="1">
         <v>165.81440000000001</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D30" s="1">
+        <v>520.98990000000003</v>
+      </c>
+      <c r="E30" s="1">
+        <v>754.10090000000002</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B31" s="1">
         <v>109.08329999999999</v>
@@ -1059,10 +1207,16 @@
       <c r="C31" s="1">
         <v>177.59270000000001</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D31" s="1">
+        <v>522.3569</v>
+      </c>
+      <c r="E31" s="1">
+        <v>766.85739999999998</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B32" s="1">
         <v>133.10810000000001</v>
@@ -1070,15 +1224,21 @@
       <c r="C32" s="1">
         <v>217.8783</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D32" s="1">
+        <v>651.85429999999997</v>
+      </c>
+      <c r="E32" s="1">
+        <v>986.66189999999995</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B34" s="1">
         <v>28.49793</v>
@@ -1086,22 +1246,28 @@
       <c r="C34" s="1">
         <v>41.394269999999999</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D34" s="1">
+        <v>257.13409999999999</v>
+      </c>
+      <c r="E34" s="1">
+        <v>326.33010000000002</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>33</v>
+      </c>
+      <c r="B35" s="1"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>34</v>
+      </c>
+      <c r="B36" s="1"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>35</v>
-      </c>
-      <c r="B35" s="1"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>36</v>
-      </c>
-      <c r="B36" s="1"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>37</v>
       </c>
       <c r="B37" s="1">
         <v>135.0359</v>
@@ -1109,10 +1275,16 @@
       <c r="C37" s="1">
         <v>172.62860000000001</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D37" s="1">
+        <v>816.16380000000004</v>
+      </c>
+      <c r="E37" s="1">
+        <v>723.58659999999998</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B38" s="1">
         <v>70.678210000000007</v>
@@ -1120,10 +1292,16 @@
       <c r="C38" s="1">
         <v>82.961209999999994</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D38" s="1">
+        <v>816.16380000000004</v>
+      </c>
+      <c r="E38" s="1">
+        <v>271.84980000000002</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B39" s="1">
         <v>51.323659999999997</v>
@@ -1131,10 +1309,11 @@
       <c r="C39" s="1">
         <v>61.53839</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E39" s="1"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B40" s="1">
         <v>71.651619999999994</v>
@@ -1142,10 +1321,16 @@
       <c r="C40" s="1">
         <v>97.600399999999993</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D40" s="1">
+        <v>318.57850000000002</v>
+      </c>
+      <c r="E40" s="1">
+        <v>271.13580000000002</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B41" s="1">
         <v>83.91686</v>
@@ -1153,10 +1338,16 @@
       <c r="C41" s="1">
         <v>99.761330000000001</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D41" s="1">
+        <v>387.27609999999999</v>
+      </c>
+      <c r="E41" s="1">
+        <v>403.84730000000002</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B42" s="1">
         <v>61.691470000000002</v>
@@ -1164,10 +1355,16 @@
       <c r="C42" s="1">
         <v>80.330359999999999</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D42" s="1">
+        <v>267.15620000000001</v>
+      </c>
+      <c r="E42" s="1">
+        <v>228.16990000000001</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B43" s="1">
         <v>65.548469999999995</v>
@@ -1175,10 +1372,16 @@
       <c r="C43" s="1">
         <v>76.320419999999999</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D43" s="1">
+        <v>290.2047</v>
+      </c>
+      <c r="E43" s="1">
+        <v>237.76070000000001</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B44" s="1">
         <v>152.70410000000001</v>
@@ -1186,10 +1389,16 @@
       <c r="C44" s="1">
         <v>238.6377</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D44" s="1">
+        <v>1249.816</v>
+      </c>
+      <c r="E44" s="1">
+        <v>1787.587</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B45" s="1">
         <v>1.2234039999999999</v>
@@ -1197,10 +1406,16 @@
       <c r="C45" s="1">
         <v>1.601129</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D45" s="1">
+        <v>5.4529350000000001</v>
+      </c>
+      <c r="E45" s="1">
+        <v>4.9245910000000004</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B46" s="1">
         <v>66.128259999999997</v>
@@ -1208,15 +1423,21 @@
       <c r="C46" s="1">
         <v>86.851240000000004</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D46" s="1">
+        <v>314.09140000000002</v>
+      </c>
+      <c r="E46" s="1">
+        <v>395.10969999999998</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B48" s="1">
         <v>272.60660000000001</v>
@@ -1224,10 +1445,16 @@
       <c r="C48" s="1">
         <v>500.755</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D48" s="1">
+        <v>1401.43</v>
+      </c>
+      <c r="E48" s="1">
+        <v>2397.4630000000002</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B49" s="1">
         <v>571.71280000000002</v>
@@ -1235,25 +1462,31 @@
       <c r="C49" s="1">
         <v>1053.829</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D49" s="1">
+        <v>3384.4870000000001</v>
+      </c>
+      <c r="E49" s="1">
+        <v>5776.0720000000001</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>51</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>53</v>
       </c>
       <c r="B53" s="1">
         <v>50.279240000000001</v>
@@ -1261,10 +1494,16 @@
       <c r="C53" s="1">
         <v>69.363870000000006</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D53" s="1">
+        <v>229.57040000000001</v>
+      </c>
+      <c r="E53" s="1">
+        <v>248.50919999999999</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B54" s="1">
         <v>6.586773</v>
@@ -1272,10 +1511,16 @@
       <c r="C54" s="1">
         <v>8.1675520000000006</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D54" s="1">
+        <v>27.777920000000002</v>
+      </c>
+      <c r="E54" s="1">
+        <v>26.469930000000002</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B55" s="1">
         <v>2.5310600000000001</v>
@@ -1283,15 +1528,26 @@
       <c r="C55" s="1">
         <v>3.23075</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D55" s="1">
+        <v>11.55226</v>
+      </c>
+      <c r="E55" s="1">
+        <v>10.419309999999999</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B58" s="1">
         <v>176.999</v>
@@ -1299,15 +1555,21 @@
       <c r="C58" s="1">
         <v>296.22399999999999</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D58" s="1">
+        <v>858.63940000000002</v>
+      </c>
+      <c r="E58" s="1">
+        <v>1477.8119999999999</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B60" s="1">
         <v>73.26388</v>
@@ -1315,10 +1577,16 @@
       <c r="C60" s="1">
         <v>89.068209999999993</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D60" s="1">
+        <v>332.6164</v>
+      </c>
+      <c r="E60" s="1">
+        <v>297.17739999999998</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B61" s="1">
         <v>0.54047610000000001</v>
@@ -1326,15 +1594,21 @@
       <c r="C61" s="1">
         <v>0.97748369999999996</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D61" s="1">
+        <v>2.8947970000000001</v>
+      </c>
+      <c r="E61" s="1">
+        <v>2.505341</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B63" s="1">
         <v>53.754869999999997</v>
@@ -1342,10 +1616,16 @@
       <c r="C63" s="1">
         <v>71.325789999999998</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D63" s="1">
+        <v>244.75149999999999</v>
+      </c>
+      <c r="E63" s="1">
+        <v>216.92949999999999</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B64" s="1">
         <v>156.4229</v>
@@ -1353,10 +1633,16 @@
       <c r="C64" s="1">
         <v>220.1628</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D64" s="1">
+        <v>1618.1220000000001</v>
+      </c>
+      <c r="E64" s="1">
+        <v>1834.31</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B65" s="1">
         <v>62.732529999999997</v>
@@ -1364,25 +1650,31 @@
       <c r="C65" s="1">
         <v>103.5214</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D65" s="1">
+        <v>293.06020000000001</v>
+      </c>
+      <c r="E65" s="1">
+        <v>388.01190000000003</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
         <v>66</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>68</v>
       </c>
       <c r="B69" s="1">
         <v>61.927630000000001</v>
@@ -1390,15 +1682,21 @@
       <c r="C69" s="1">
         <v>109.2349</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D69" s="1">
+        <v>291.99880000000002</v>
+      </c>
+      <c r="E69" s="1">
+        <v>271.34339999999997</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B71" s="1">
         <v>71.936040000000006</v>
@@ -1406,10 +1704,16 @@
       <c r="C71" s="1">
         <v>99.285939999999997</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D71" s="1">
+        <v>377.75389999999999</v>
+      </c>
+      <c r="E71" s="1">
+        <v>481.31169999999997</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B72" s="1">
         <v>99.207520000000002</v>
@@ -1417,10 +1721,16 @@
       <c r="C72" s="1">
         <v>140.4485</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D72" s="1">
+        <v>377.75389999999999</v>
+      </c>
+      <c r="E72" s="1">
+        <v>661.61469999999997</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B73" s="1">
         <v>97.236980000000003</v>
@@ -1428,15 +1738,21 @@
       <c r="C73" s="1">
         <v>140.11429999999999</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D73" s="1">
+        <v>524.84130000000005</v>
+      </c>
+      <c r="E73" s="1">
+        <v>664.50940000000003</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B75" s="1">
         <v>10.95966</v>
@@ -1444,10 +1760,16 @@
       <c r="C75" s="1">
         <v>9.5988140000000008</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D75" s="1">
+        <v>10.181990000000001</v>
+      </c>
+      <c r="E75" s="1">
+        <v>9.8691639999999996</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B76" s="1">
         <v>36.859630000000003</v>
@@ -1456,9 +1778,9 @@
         <v>51.214179999999999</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B77" s="1">
         <v>54.122619999999998</v>
@@ -1466,10 +1788,16 @@
       <c r="C77" s="1">
         <v>74.611490000000003</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D77" s="1">
+        <v>272.7878</v>
+      </c>
+      <c r="E77" s="1">
+        <v>288.83449999999999</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B78" s="1">
         <v>201.55170000000001</v>
@@ -1477,10 +1805,16 @@
       <c r="C78" s="1">
         <v>195.4041</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D78" s="1">
+        <v>330.392</v>
+      </c>
+      <c r="E78" s="1">
+        <v>307.67430000000002</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B79" s="1">
         <v>88.047799999999995</v>
@@ -1488,10 +1822,16 @@
       <c r="C79" s="1">
         <v>115.1658</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D79" s="1">
+        <v>458.35759999999999</v>
+      </c>
+      <c r="E79" s="1">
+        <v>485.19310000000002</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B80" s="1">
         <v>64.768659999999997</v>
@@ -1499,10 +1839,16 @@
       <c r="C80" s="1">
         <v>96.694230000000005</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D80" s="1">
+        <v>322.27879999999999</v>
+      </c>
+      <c r="E80" s="1">
+        <v>312.72239999999999</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B81" s="1">
         <v>48.85445</v>
@@ -1511,9 +1857,9 @@
         <v>70.637709999999998</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B82" s="1">
         <v>67.121769999999998</v>
@@ -1521,16 +1867,22 @@
       <c r="C82" s="1">
         <v>88.43674</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D82" s="1">
+        <v>302.38</v>
+      </c>
+      <c r="E82" s="1">
+        <v>275.06569999999999</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B83" s="1"/>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B84" s="1">
         <v>1.605707</v>
@@ -1538,15 +1890,21 @@
       <c r="C84" s="1">
         <v>2.081226</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D84" s="1">
+        <v>10.66192</v>
+      </c>
+      <c r="E84" s="1">
+        <v>10.432869999999999</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B86" s="1">
         <v>286.55259999999998</v>
@@ -1554,10 +1912,16 @@
       <c r="C86" s="1">
         <v>284.81959999999998</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D86" s="1">
+        <v>316.79399999999998</v>
+      </c>
+      <c r="E86" s="1">
+        <v>307.11270000000002</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B87" s="1">
         <v>366.49900000000002</v>
@@ -1565,10 +1929,16 @@
       <c r="C87" s="1">
         <v>359.13240000000002</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D87" s="1">
+        <v>405.59289999999999</v>
+      </c>
+      <c r="E87" s="1">
+        <v>396.57830000000001</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B88" s="1">
         <v>144.35339999999999</v>
@@ -1576,10 +1946,16 @@
       <c r="C88" s="1">
         <v>157.24</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D88" s="1">
+        <v>366.27390000000003</v>
+      </c>
+      <c r="E88" s="1">
+        <v>366.57769999999999</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B89" s="1">
         <v>11.414899999999999</v>
@@ -1587,10 +1963,16 @@
       <c r="C89" s="1">
         <v>10.380549999999999</v>
       </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D89" s="1">
+        <v>5.8871250000000002</v>
+      </c>
+      <c r="E89" s="1">
+        <v>5.9571550000000002</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B90" s="1">
         <v>921.88530000000003</v>
@@ -1598,10 +1980,16 @@
       <c r="C90" s="1">
         <v>1284</v>
       </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D90" s="1">
+        <v>451.4171</v>
+      </c>
+      <c r="E90" s="1">
+        <v>635.82569999999998</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B91" s="1">
         <v>914.11210000000005</v>
@@ -1609,10 +1997,16 @@
       <c r="C91" s="1">
         <v>1444.2829999999999</v>
       </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D91" s="1">
+        <v>2877.57</v>
+      </c>
+      <c r="E91" s="1">
+        <v>4248.8599999999997</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B92" s="1">
         <v>57.713790000000003</v>
@@ -1620,10 +2014,16 @@
       <c r="C92" s="1">
         <v>78.883769999999998</v>
       </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D92" s="1">
+        <v>2877.57</v>
+      </c>
+      <c r="E92" s="1">
+        <v>280.27629999999999</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B93" s="1">
         <v>1.229061</v>
@@ -1631,10 +2031,16 @@
       <c r="C93" s="1">
         <v>1.7108490000000001</v>
       </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D93" s="1">
+        <v>6.1999170000000001</v>
+      </c>
+      <c r="E93" s="1">
+        <v>4.3478320000000004</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B94" s="1">
         <v>82.849789999999999</v>
@@ -1642,10 +2048,16 @@
       <c r="C94" s="1">
         <v>121.0333</v>
       </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D94" s="1">
+        <v>422.822</v>
+      </c>
+      <c r="E94" s="1">
+        <v>524.36159999999995</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B95" s="1">
         <v>56.017949999999999</v>
@@ -1653,10 +2065,16 @@
       <c r="C95" s="1">
         <v>76.542190000000005</v>
       </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D95" s="1">
+        <v>261.18939999999998</v>
+      </c>
+      <c r="E95" s="1">
+        <v>263.52069999999998</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B96" s="1">
         <v>49.906379999999999</v>
@@ -1664,10 +2082,16 @@
       <c r="C96" s="1">
         <v>68.152540000000002</v>
       </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D96" s="1">
+        <v>235.77690000000001</v>
+      </c>
+      <c r="E96" s="1">
+        <v>218.3595</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B97" s="1">
         <v>0.83431770000000005</v>
@@ -1675,10 +2099,16 @@
       <c r="C97" s="1">
         <v>1.367942</v>
       </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D97" s="1">
+        <v>3.978396</v>
+      </c>
+      <c r="E97" s="1">
+        <v>4.4309269999999996</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B98" s="1">
         <v>3230.395</v>
@@ -1686,10 +2116,16 @@
       <c r="C98" s="1">
         <v>5820.732</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D98" s="1">
+        <v>16109.57</v>
+      </c>
+      <c r="E98" s="1">
+        <v>22008.62</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B99" s="1">
         <v>239.56620000000001</v>
@@ -1697,10 +2133,16 @@
       <c r="C99" s="1">
         <v>372.91590000000002</v>
       </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D99" s="1">
+        <v>1809.779</v>
+      </c>
+      <c r="E99" s="1">
+        <v>2119.0740000000001</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B100" s="1">
         <v>2.3055599999999998</v>
@@ -1708,10 +2150,16 @@
       <c r="C100" s="1">
         <v>3.188132</v>
       </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D100" s="1">
+        <v>11.0246</v>
+      </c>
+      <c r="E100" s="1">
+        <v>10.59539</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B101" s="1">
         <v>238.38249999999999</v>
@@ -1719,17 +2167,23 @@
       <c r="C101" s="1">
         <v>371.47230000000002</v>
       </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D101" s="1">
+        <v>1807.9079999999999</v>
+      </c>
+      <c r="E101" s="1">
+        <v>2135.9899999999998</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B103" s="1">
         <v>5.8464039999999997</v>
@@ -1737,10 +2191,16 @@
       <c r="C103" s="1">
         <v>4.8076489999999996</v>
       </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D103" s="1">
+        <v>7.5252790000000003</v>
+      </c>
+      <c r="E103" s="1">
+        <v>7.6736329999999997</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B104" s="1">
         <v>182.65049999999999</v>
@@ -1748,10 +2208,16 @@
       <c r="C104" s="1">
         <v>257.26560000000001</v>
       </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D104" s="1">
+        <v>352.35300000000001</v>
+      </c>
+      <c r="E104" s="1">
+        <v>424.53699999999998</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B105" s="1">
         <v>4.4165469999999996</v>
@@ -1759,15 +2225,21 @@
       <c r="C105" s="1">
         <v>6.2838960000000004</v>
       </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D105" s="1">
+        <v>16.455010000000001</v>
+      </c>
+      <c r="E105" s="1">
+        <v>20.715409999999999</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B107" s="1">
         <v>2.5066860000000002</v>
@@ -1775,10 +2247,16 @@
       <c r="C107" s="1">
         <v>4.0316609999999997</v>
       </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D107" s="1">
+        <v>11.30087</v>
+      </c>
+      <c r="E107" s="1">
+        <v>12.14363</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B108" s="1">
         <v>65.589420000000004</v>
@@ -1786,10 +2264,16 @@
       <c r="C108" s="1">
         <v>99.530789999999996</v>
       </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D108" s="1">
+        <v>334.60270000000003</v>
+      </c>
+      <c r="E108" s="1">
+        <v>382.72629999999998</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B109" s="1">
         <v>80.267049999999998</v>
@@ -1797,10 +2281,16 @@
       <c r="C109" s="1">
         <v>121.0615</v>
       </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D109" s="1">
+        <v>391.71600000000001</v>
+      </c>
+      <c r="E109" s="1">
+        <v>448.54880000000003</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B110" s="1">
         <v>430.7731</v>
@@ -1808,10 +2298,16 @@
       <c r="C110" s="1">
         <v>585.43039999999996</v>
       </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D110" s="1">
+        <v>453.69040000000001</v>
+      </c>
+      <c r="E110" s="1">
+        <v>448.54880000000003</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B111" s="1">
         <v>434.03930000000003</v>
@@ -1819,10 +2315,16 @@
       <c r="C111" s="1">
         <v>585.43039999999996</v>
       </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D111" s="1">
+        <v>453.5548</v>
+      </c>
+      <c r="E111" s="1">
+        <v>553.58950000000004</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B112" s="1">
         <v>73.104320000000001</v>
@@ -1830,10 +2332,16 @@
       <c r="C112" s="1">
         <v>105.91459999999999</v>
       </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D112" s="1">
+        <v>345.17469999999997</v>
+      </c>
+      <c r="E112" s="1">
+        <v>345.3673</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B113" s="1">
         <v>186.27449999999999</v>
@@ -1842,9 +2350,9 @@
         <v>330.0104</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B114" s="1">
         <v>173.93879999999999</v>
@@ -1852,10 +2360,16 @@
       <c r="C114" s="1">
         <v>287.8109</v>
       </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D114" s="1">
+        <v>1081.211</v>
+      </c>
+      <c r="E114" s="1">
+        <v>1196.364</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B115" s="1">
         <v>17.350249999999999</v>
@@ -1863,10 +2377,16 @@
       <c r="C115" s="1">
         <v>30.527660000000001</v>
       </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D115" s="1">
+        <v>87.592290000000006</v>
+      </c>
+      <c r="E115" s="1">
+        <v>102.45269999999999</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B116" s="1">
         <v>335.2439</v>
@@ -1874,10 +2394,16 @@
       <c r="C116" s="1">
         <v>567.04070000000002</v>
       </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D116" s="1">
+        <v>1901.28</v>
+      </c>
+      <c r="E116" s="1">
+        <v>2242.2840000000001</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B117" s="1">
         <v>93.002160000000003</v>
@@ -1885,10 +2411,16 @@
       <c r="C117" s="1">
         <v>176.84370000000001</v>
       </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D117" s="1">
+        <v>500.71519999999998</v>
+      </c>
+      <c r="E117" s="1">
+        <v>728.17150000000004</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B118" s="1">
         <v>35.273780000000002</v>
@@ -1896,10 +2428,16 @@
       <c r="C118" s="1">
         <v>57.031970000000001</v>
       </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D118" s="1">
+        <v>166.16679999999999</v>
+      </c>
+      <c r="E118" s="1">
+        <v>187.3921</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B119" s="1">
         <v>76.734809999999996</v>
@@ -1907,10 +2445,16 @@
       <c r="C119" s="1">
         <v>125.642</v>
       </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D119" s="1">
+        <v>362.24930000000001</v>
+      </c>
+      <c r="E119" s="1">
+        <v>391.56849999999997</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B120" s="1">
         <v>37.238019999999999</v>
@@ -1918,10 +2462,16 @@
       <c r="C120" s="1">
         <v>57.813490000000002</v>
       </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D120" s="1">
+        <v>163.92740000000001</v>
+      </c>
+      <c r="E120" s="1">
+        <v>205.6866</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B121" s="1">
         <v>63.768000000000001</v>
@@ -1929,10 +2479,16 @@
       <c r="C121" s="1">
         <v>99.179270000000002</v>
       </c>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D121" s="1">
+        <v>289.4051</v>
+      </c>
+      <c r="E121" s="1">
+        <v>287.89640000000003</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B122" s="1">
         <v>78.638109999999998</v>
@@ -1940,10 +2496,16 @@
       <c r="C122" s="1">
         <v>121.0194</v>
       </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D122" s="1">
+        <v>376.2269</v>
+      </c>
+      <c r="E122" s="1">
+        <v>401.02409999999998</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B123" s="1">
         <v>77.926199999999994</v>
@@ -1951,16 +2513,22 @@
       <c r="C123" s="1">
         <v>125.9353</v>
       </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D123" s="1">
+        <v>383.8972</v>
+      </c>
+      <c r="E123" s="1">
+        <v>468.85629999999998</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B124" s="1"/>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B125" s="1">
         <v>78.796660000000003</v>
@@ -1968,10 +2536,16 @@
       <c r="C125" s="1">
         <v>120.57210000000001</v>
       </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D125" s="1">
+        <v>359.66460000000001</v>
+      </c>
+      <c r="E125" s="1">
+        <v>370.99489999999997</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B126" s="1">
         <v>1.4055629999999999</v>
@@ -1980,9 +2554,9 @@
         <v>0.70941370000000004</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>